<commit_message>
Graficas y datos no obligatorios
</commit_message>
<xml_diff>
--- a/ventas.xlsx
+++ b/ventas.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Muestra de los productos</t>
   </si>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t>JKL-012</t>
+  </si>
+  <si>
+    <t>Gorra</t>
   </si>
   <si>
     <t>Total</t>
@@ -73,7 +76,7 @@
     <font>
       <b/>
       <sz val="24"/>
-      <color rgb="FF333333"/>
+      <color rgb="FF0000CD"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -191,6 +194,400 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Ventas por producto</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="1E90FF"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="DC143C"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="006400"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF8C00"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>productos!$C$5:$C$9</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Blusa azul</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Zapatos negros</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Sombrero claro</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Lentes oscuros</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Gorra</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>productos!$F$5:$F$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>255</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>378</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>499.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>768</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>80.36</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="50010001"/>
+        <c:axId val="50010002"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="50010001"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Nombre del producto</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50010002"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="50010002"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Precio</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="$#,##0.00" sourceLinked="0"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50010001"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Gráfica de pastel</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Gráfica de pastel</c:v>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="1E90FF"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="DC143C"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="006400"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF8C00"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>productos!$C$5:$C$9</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Blusa azul</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Zapatos negros</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Sombrero claro</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Lentes oscuros</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Gorra</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>productos!$F$5:$F$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>255</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>378</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>499.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>768</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>80.36</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -478,10 +875,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr>
-    <tabColor rgb="FFFFFFFF"/>
-  </sheetPr>
-  <dimension ref="A1:BS9"/>
+  <dimension ref="A1:BS10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -495,13 +889,16 @@
     <col min="7" max="71" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:6" s="1" customFormat="1"/>
-    <row r="2" spans="3:6">
+    <row r="1" spans="3:8" s="1" customFormat="1"/>
+    <row r="2" spans="3:8">
+      <c r="E2" s="2"/>
       <c r="F2" s="2" t="s">
         <v>0</v>
       </c>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
     </row>
-    <row r="4" spans="3:6">
+    <row r="4" spans="3:8">
       <c r="C4" s="3" t="s">
         <v>1</v>
       </c>
@@ -515,7 +912,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="3:6">
+    <row r="5" spans="3:8">
       <c r="C5" s="4" t="s">
         <v>5</v>
       </c>
@@ -529,7 +926,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="6" spans="3:6">
+    <row r="6" spans="3:8">
       <c r="C6" s="4" t="s">
         <v>7</v>
       </c>
@@ -543,7 +940,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="7" spans="3:6">
+    <row r="7" spans="3:8">
       <c r="C7" s="4" t="s">
         <v>9</v>
       </c>
@@ -557,7 +954,7 @@
         <v>499.9</v>
       </c>
     </row>
-    <row r="8" spans="3:6">
+    <row r="8" spans="3:8">
       <c r="C8" s="4" t="s">
         <v>11</v>
       </c>
@@ -571,15 +968,26 @@
         <v>768</v>
       </c>
     </row>
-    <row r="9" spans="3:6">
-      <c r="E9" s="5" t="s">
+    <row r="9" spans="3:8">
+      <c r="C9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="5">
-        <v>1900.9</v>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4">
+        <v>80.36</v>
+      </c>
+    </row>
+    <row r="10" spans="3:8">
+      <c r="E10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="5">
+        <v>1981.26</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Agregar hora y fecha al documento
</commit_message>
<xml_diff>
--- a/ventas.xlsx
+++ b/ventas.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Muestra de los productos</t>
   </si>
@@ -29,6 +29,18 @@
   </si>
   <si>
     <t>Precio del producto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fecha en que se generó el reporte: </t>
+  </si>
+  <si>
+    <t>2023/05/16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hora en que se generó el reporte: </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 15:43</t>
   </si>
   <si>
     <t>Blusa azul</t>
@@ -300,7 +312,7 @@
                   <c:v>768</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>80.36</c:v>
+                  <c:v>127.35</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -492,7 +504,7 @@
                   <c:v>768</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>80.36</c:v>
+                  <c:v>127.35</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -565,8 +577,8 @@
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
@@ -886,19 +898,36 @@
     <col min="4" max="4" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="71" width="9.140625" style="1"/>
+    <col min="7" max="9" width="9.140625" style="1"/>
+    <col min="10" max="10" width="32.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="71" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:8" s="1" customFormat="1"/>
-    <row r="2" spans="3:8">
+    <row r="1" spans="3:11" s="1" customFormat="1"/>
+    <row r="2" spans="3:11">
       <c r="E2" s="2"/>
       <c r="F2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
+      <c r="J2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="4" spans="3:8">
+    <row r="3" spans="3:11">
+      <c r="J3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="3:11">
       <c r="C4" s="3" t="s">
         <v>1</v>
       </c>
@@ -912,78 +941,78 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="3:8">
+    <row r="5" spans="3:11">
       <c r="C5" s="4" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D5" s="4">
         <v>1</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F5" s="4">
         <v>255</v>
       </c>
     </row>
-    <row r="6" spans="3:8">
+    <row r="6" spans="3:11">
       <c r="C6" s="4" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D6" s="4">
         <v>2</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F6" s="4">
         <v>378</v>
       </c>
     </row>
-    <row r="7" spans="3:8">
+    <row r="7" spans="3:11">
       <c r="C7" s="4" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D7" s="4">
         <v>3</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F7" s="4">
         <v>499.9</v>
       </c>
     </row>
-    <row r="8" spans="3:8">
+    <row r="8" spans="3:11">
       <c r="C8" s="4" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D8" s="4">
         <v>4</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="F8" s="4">
         <v>768</v>
       </c>
     </row>
-    <row r="9" spans="3:8">
+    <row r="9" spans="3:11">
       <c r="C9" s="4" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4">
-        <v>80.36</v>
+        <v>127.35</v>
       </c>
     </row>
-    <row r="10" spans="3:8">
+    <row r="10" spans="3:11">
       <c r="E10" s="5" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F10" s="5">
-        <v>1981.26</v>
+        <v>2028.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Inicio de replica excel PM
</commit_message>
<xml_diff>
--- a/ventas.xlsx
+++ b/ventas.xlsx
@@ -28,19 +28,19 @@
     <t>SKU del producto</t>
   </si>
   <si>
-    <t>Precio del producto</t>
+    <t>Precio del productooooooo</t>
   </si>
   <si>
     <t xml:space="preserve">Fecha en que se generó el reporte: </t>
   </si>
   <si>
-    <t>2023/05/17</t>
+    <t>2023/05/19</t>
   </si>
   <si>
     <t xml:space="preserve">Hora en que se generó el reporte: </t>
   </si>
   <si>
-    <t xml:space="preserve"> 14:36</t>
+    <t xml:space="preserve"> 15:18</t>
   </si>
   <si>
     <t>Blusa azul</t>
@@ -548,7 +548,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
+      <xdr:colOff>371475</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -887,7 +887,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BS10"/>
+  <dimension ref="A1:CW10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -897,11 +897,11 @@
     <col min="3" max="3" width="20" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="9" width="9.140625" style="1"/>
     <col min="10" max="10" width="32.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="71" width="9.140625" style="1"/>
+    <col min="12" max="101" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="3:11" s="1" customFormat="1"/>

</xml_diff>